<commit_message>
results from 10000 iters
</commit_message>
<xml_diff>
--- a/IBpil_scenarios.xlsx
+++ b/IBpil_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Use\GitHub\IBpil_mse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69CC12A-9E8C-46A8-A2D9-10F2F1935635}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719D7273-B845-4AAA-A2D1-3A9BEAB53113}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,8 +553,8 @@
   <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1739,13 +1739,13 @@
       </c>
       <c r="B38" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSss3_HCR12_REClow_INNvar_OERnaq</v>
+        <v>ASSss3_HCR13_REClow_INNvar_OERnaq</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>7</v>
@@ -1780,13 +1780,13 @@
       </c>
       <c r="B39" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSss3_HCR12_REClowmed_INNvar_OERnaq</v>
+        <v>ASSss3_HCR13_REClowmed_INNvar_OERnaq</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>12</v>
@@ -1816,13 +1816,13 @@
       </c>
       <c r="B40" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSss3_HCR12_RECmix_INNvar_OERnaq</v>
+        <v>ASSss3_HCR13_RECmix_INNvar_OERnaq</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>13</v>
@@ -1854,13 +1854,13 @@
       </c>
       <c r="B41" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSnone_HCR12_REClow_INNvar_OERnone</v>
+        <v>ASSnone_HCR13_REClow_INNvar_OERnone</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>7</v>
@@ -1886,13 +1886,13 @@
       </c>
       <c r="B42" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSnone_HCR12_REClowmed_INNvar_OERnone</v>
+        <v>ASSnone_HCR13_REClowmed_INNvar_OERnone</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>12</v>
@@ -1918,13 +1918,13 @@
       </c>
       <c r="B43" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSnone_HCR12_RECmix_INNvar_OERnone</v>
+        <v>ASSnone_HCR13_RECmix_INNvar_OERnone</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
code new rules (TACmax 35 and 30 kt)
</commit_message>
<xml_diff>
--- a/IBpil_scenarios.xlsx
+++ b/IBpil_scenarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Use\GitHub\IBpil_mse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719D7273-B845-4AAA-A2D1-3A9BEAB53113}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BACF43E-67FE-4484-9392-5F61AA521384}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="41">
   <si>
     <t>Scenario</t>
   </si>
@@ -184,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +200,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,7 +233,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -263,6 +269,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -550,11 +562,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -641,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="str">
-        <f t="shared" ref="B3:B43" si="0">CONCATENATE("ASS",C3,"_HCR",D3,"_REC",E3,"_INN",F3,"_OER",G3)</f>
+        <f t="shared" ref="B3:B56" si="0">CONCATENATE("ASS",C3,"_HCR",D3,"_REC",E3,"_INN",F3,"_OER",G3)</f>
         <v>ASSss3_HCR9_REClow_INNvar_OERnaq</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1329,7 +1341,7 @@
       <c r="H26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="K26" s="14" t="s">
         <v>15</v>
       </c>
       <c r="L26" s="7" t="s">
@@ -1368,7 +1380,7 @@
       <c r="H27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K27" s="12"/>
+      <c r="K27" s="14"/>
       <c r="L27" s="7" t="s">
         <v>17</v>
       </c>
@@ -1408,7 +1420,7 @@
       <c r="J28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="12"/>
+      <c r="K28" s="14"/>
       <c r="L28" s="7" t="s">
         <v>18</v>
       </c>
@@ -1448,7 +1460,7 @@
       <c r="H29" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K29" s="12"/>
+      <c r="K29" s="14"/>
       <c r="P29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1479,7 +1491,7 @@
       <c r="H30" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K30" s="12"/>
+      <c r="K30" s="14"/>
       <c r="P30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1513,7 +1525,7 @@
       <c r="J31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="12"/>
+      <c r="K31" s="14"/>
       <c r="P31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1544,7 +1556,7 @@
       <c r="H32" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K32" s="12" t="s">
+      <c r="K32" s="14" t="s">
         <v>19</v>
       </c>
       <c r="L32" s="7" t="s">
@@ -1583,7 +1595,7 @@
       <c r="H33" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K33" s="12"/>
+      <c r="K33" s="14"/>
       <c r="L33" s="7" t="s">
         <v>17</v>
       </c>
@@ -1623,7 +1635,7 @@
       <c r="J34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K34" s="12"/>
+      <c r="K34" s="14"/>
       <c r="L34" s="7" t="s">
         <v>18</v>
       </c>
@@ -1663,7 +1675,7 @@
       <c r="H35" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K35" s="12"/>
+      <c r="K35" s="14"/>
       <c r="P35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1694,7 +1706,7 @@
       <c r="H36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K36" s="12"/>
+      <c r="K36" s="14"/>
       <c r="P36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1728,7 +1740,7 @@
       <c r="J37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K37" s="12"/>
+      <c r="K37" s="14"/>
       <c r="P37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1737,220 +1749,560 @@
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="str">
+      <c r="B38" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ASSss3_HCR13_REClow_INNvar_OERnaq</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="6">
         <v>13</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="6" t="s">
+      <c r="E38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M38" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="12"/>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="str">
+      <c r="B39" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ASSss3_HCR13_REClowmed_INNvar_OERnaq</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="6">
         <v>13</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="6" t="s">
+      <c r="F39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M39" s="10">
-        <v>196334</v>
-      </c>
+      <c r="J39" s="5"/>
+      <c r="K39" s="12"/>
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="str">
+      <c r="B40" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ASSss3_HCR13_RECmix_INNvar_OERnaq</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="6">
         <v>13</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="6" t="s">
+      <c r="E40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I40" s="9"/>
-      <c r="J40" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K40" s="13"/>
-      <c r="L40" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="M40" s="10">
-        <v>252523</v>
-      </c>
+      <c r="J40" s="5"/>
+      <c r="K40" s="12"/>
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="str">
+      <c r="B41" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ASSnone_HCR13_REClow_INNvar_OERnone</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="6">
         <v>13</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G41" s="9" t="s">
+      <c r="E41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="12"/>
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="8" t="str">
+      <c r="B42" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ASSnone_HCR13_REClowmed_INNvar_OERnone</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="6">
         <v>13</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="9" t="s">
+      <c r="F42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="12"/>
     </row>
     <row r="43" spans="1:16">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="8" t="str">
+      <c r="B43" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ASSnone_HCR13_RECmix_INNvar_OERnone</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="6">
         <v>13</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" s="9" t="s">
+      <c r="E43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I43" s="9"/>
-      <c r="J43" s="6" t="s">
+      <c r="J43" s="5"/>
+      <c r="K43" s="12"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSss3_HCR14_REClow_INNvar_OERnaq</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="6">
         <v>14</v>
       </c>
-      <c r="K43" s="13"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
+      <c r="E44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J44" s="5"/>
+      <c r="K44" s="12"/>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSss3_HCR14_REClowmed_INNvar_OERnaq</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="6">
+        <v>14</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J45" s="5"/>
+      <c r="K45" s="12"/>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSss3_HCR14_RECmix_INNvar_OERnaq</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="6">
+        <v>14</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J46" s="5"/>
+      <c r="K46" s="12"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSnone_HCR14_REClow_INNvar_OERnone</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="6">
+        <v>14</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J47" s="5"/>
+      <c r="K47" s="12"/>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSnone_HCR14_REClowmed_INNvar_OERnone</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="6">
+        <v>14</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="12"/>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSnone_HCR14_RECmix_INNvar_OERnone</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="6">
+        <v>14</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J49" s="5"/>
+      <c r="K49" s="12"/>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="12"/>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="B51" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSss3_HCR15_REClow_INNvar_OERnaq</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="13">
+        <v>15</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L51" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="B52" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSss3_HCR15_REClowmed_INNvar_OERnaq</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="13">
+        <v>15</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M52" s="10">
+        <v>196334</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="B53" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSss3_HCR15_RECmix_INNvar_OERnaq</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="13">
+        <v>15</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I53" s="9"/>
+      <c r="J53" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K53" s="15"/>
+      <c r="L53" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M53" s="10">
+        <v>252523</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="B54" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSnone_HCR15_REClow_INNvar_OERnone</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="13">
+        <v>15</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="B55" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSnone_HCR15_REClowmed_INNvar_OERnone</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="13">
+        <v>15</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="B56" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>ASSnone_HCR15_RECmix_INNvar_OERnone</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="13">
+        <v>15</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I56" s="9"/>
+      <c r="J56" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K56" s="15"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="K26:K31"/>
     <mergeCell ref="K32:K37"/>
-    <mergeCell ref="K38:K43"/>
+    <mergeCell ref="K51:K56"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update code for calculation of refpts (rules with Btrigger)
</commit_message>
<xml_diff>
--- a/IBpil_scenarios.xlsx
+++ b/IBpil_scenarios.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Use\GitHub\IBpil_mse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BACF43E-67FE-4484-9392-5F61AA521384}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220DBEB5-2A4B-4B34-926F-806FD6535E09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="rules_for_refpts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="48">
   <si>
     <t>Scenario</t>
   </si>
@@ -154,18 +155,46 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Rule12</t>
+  </si>
+  <si>
+    <t>F fixed</t>
+  </si>
+  <si>
+    <t>Rule15</t>
+  </si>
+  <si>
+    <t>ICES AR with varying F and Blim and MSYBtrigger from low regime</t>
+  </si>
+  <si>
+    <t>Rule16</t>
+  </si>
+  <si>
+    <t>ICES AR with varying F and Blim and MSYBtrigger from medium regime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -237,50 +266,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,9 +593,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M33" sqref="M33:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1341,7 +1370,7 @@
       <c r="H26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="14" t="s">
+      <c r="K26" s="13" t="s">
         <v>15</v>
       </c>
       <c r="L26" s="7" t="s">
@@ -1380,7 +1409,7 @@
       <c r="H27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K27" s="14"/>
+      <c r="K27" s="13"/>
       <c r="L27" s="7" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1449,7 @@
       <c r="J28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="14"/>
+      <c r="K28" s="13"/>
       <c r="L28" s="7" t="s">
         <v>18</v>
       </c>
@@ -1460,7 +1489,7 @@
       <c r="H29" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K29" s="14"/>
+      <c r="K29" s="13"/>
       <c r="P29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1491,7 +1520,7 @@
       <c r="H30" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K30" s="14"/>
+      <c r="K30" s="13"/>
       <c r="P30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1525,7 +1554,7 @@
       <c r="J31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="14"/>
+      <c r="K31" s="13"/>
       <c r="P31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1556,7 +1585,7 @@
       <c r="H32" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="13" t="s">
         <v>19</v>
       </c>
       <c r="L32" s="7" t="s">
@@ -1595,7 +1624,7 @@
       <c r="H33" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K33" s="14"/>
+      <c r="K33" s="13"/>
       <c r="L33" s="7" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1664,7 @@
       <c r="J34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K34" s="14"/>
+      <c r="K34" s="13"/>
       <c r="L34" s="7" t="s">
         <v>18</v>
       </c>
@@ -1675,7 +1704,7 @@
       <c r="H35" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K35" s="14"/>
+      <c r="K35" s="13"/>
       <c r="P35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1706,7 +1735,7 @@
       <c r="H36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K36" s="14"/>
+      <c r="K36" s="13"/>
       <c r="P36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1740,7 +1769,7 @@
       <c r="J37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K37" s="14"/>
+      <c r="K37" s="13"/>
       <c r="P37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2106,13 +2135,13 @@
     <row r="51" spans="1:16">
       <c r="B51" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSss3_HCR15_REClow_INNvar_OERnaq</v>
+        <v>ASSss3_HCR??_REClow_INNvar_OERnaq</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="13">
-        <v>15</v>
+      <c r="D51" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>7</v>
@@ -2128,7 +2157,7 @@
       </c>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
-      <c r="K51" s="15" t="s">
+      <c r="K51" s="14" t="s">
         <v>20</v>
       </c>
       <c r="L51" s="10" t="s">
@@ -2144,13 +2173,13 @@
     <row r="52" spans="1:16">
       <c r="B52" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSss3_HCR15_REClowmed_INNvar_OERnaq</v>
+        <v>ASSss3_HCR??_REClowmed_INNvar_OERnaq</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="13">
-        <v>15</v>
+      <c r="D52" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>12</v>
@@ -2166,7 +2195,7 @@
       </c>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
-      <c r="K52" s="15"/>
+      <c r="K52" s="14"/>
       <c r="L52" s="10" t="s">
         <v>17</v>
       </c>
@@ -2177,13 +2206,13 @@
     <row r="53" spans="1:16">
       <c r="B53" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSss3_HCR15_RECmix_INNvar_OERnaq</v>
+        <v>ASSss3_HCR??_RECmix_INNvar_OERnaq</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="13">
-        <v>15</v>
+      <c r="D53" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>13</v>
@@ -2201,7 +2230,7 @@
       <c r="J53" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K53" s="15"/>
+      <c r="K53" s="14"/>
       <c r="L53" s="10" t="s">
         <v>18</v>
       </c>
@@ -2212,13 +2241,13 @@
     <row r="54" spans="1:16">
       <c r="B54" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSnone_HCR15_REClow_INNvar_OERnone</v>
+        <v>ASSnone_HCR??_REClow_INNvar_OERnone</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="13">
-        <v>15</v>
+      <c r="D54" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>7</v>
@@ -2234,20 +2263,20 @@
       </c>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
-      <c r="K54" s="15"/>
+      <c r="K54" s="14"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
     </row>
     <row r="55" spans="1:16">
       <c r="B55" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSnone_HCR15_REClowmed_INNvar_OERnone</v>
+        <v>ASSnone_HCR??_REClowmed_INNvar_OERnone</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="13">
-        <v>15</v>
+      <c r="D55" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>12</v>
@@ -2263,20 +2292,20 @@
       </c>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
-      <c r="K55" s="15"/>
+      <c r="K55" s="14"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
     </row>
     <row r="56" spans="1:16">
       <c r="B56" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ASSnone_HCR15_RECmix_INNvar_OERnone</v>
+        <v>ASSnone_HCR??_RECmix_INNvar_OERnone</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="13">
-        <v>15</v>
+      <c r="D56" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>13</v>
@@ -2294,7 +2323,7 @@
       <c r="J56" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K56" s="15"/>
+      <c r="K56" s="14"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
     </row>
@@ -2307,4 +2336,44 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A98D134-9AF6-4269-8120-60C2C27FE276}">
+  <dimension ref="B3:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>